<commit_message>
color code and order updated for Showroom
</commit_message>
<xml_diff>
--- a/CSV-Data/SubOccupancyCodeList.xlsx
+++ b/CSV-Data/SubOccupancyCodeList.xlsx
@@ -1065,7 +1065,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1087,12 +1087,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1137,7 +1131,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1151,10 +1145,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1181,8 +1171,8 @@
   </sheetPr>
   <dimension ref="A1:J162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2585,7 +2575,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
@@ -2618,7 +2608,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>100</v>
       </c>
@@ -2652,7 +2642,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -2665,6 +2655,18 @@
       <c r="D45" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="E45" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>29</v>
+      </c>
       <c r="I45" s="1" t="s">
         <v>102</v>
       </c>
@@ -2672,7 +2674,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>104</v>
       </c>
@@ -2696,7 +2698,7 @@
         <v>47</v>
       </c>
       <c r="H46" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>104</v>
@@ -2705,7 +2707,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>106</v>
       </c>
@@ -2729,7 +2731,7 @@
         <v>48</v>
       </c>
       <c r="H47" s="1" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>106</v>
@@ -2738,7 +2740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>108</v>
       </c>
@@ -2762,7 +2764,7 @@
         <v>49</v>
       </c>
       <c r="H48" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>108</v>
@@ -2771,7 +2773,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>110</v>
       </c>
@@ -2795,7 +2797,7 @@
         <v>50</v>
       </c>
       <c r="H49" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>110</v>
@@ -2804,7 +2806,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>112</v>
       </c>
@@ -2828,7 +2830,7 @@
         <v>51</v>
       </c>
       <c r="H50" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>112</v>
@@ -2837,7 +2839,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>114</v>
       </c>
@@ -2861,7 +2863,7 @@
         <v>52</v>
       </c>
       <c r="H51" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>114</v>
@@ -2870,7 +2872,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>116</v>
       </c>
@@ -2894,7 +2896,7 @@
         <v>53</v>
       </c>
       <c r="H52" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>116</v>
@@ -2903,7 +2905,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>118</v>
       </c>
@@ -2927,7 +2929,7 @@
         <v>54</v>
       </c>
       <c r="H53" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>118</v>
@@ -2936,7 +2938,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>120</v>
       </c>
@@ -2960,7 +2962,7 @@
         <v>55</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>120</v>
@@ -2969,7 +2971,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>122</v>
       </c>
@@ -2993,7 +2995,7 @@
         <v>56</v>
       </c>
       <c r="H55" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>122</v>

</xml_diff>